<commit_message>
Add support for organizations description translation
</commit_message>
<xml_diff>
--- a/RAWImporter/data/monthly example.xlsx
+++ b/RAWImporter/data/monthly example.xlsx
@@ -41,10 +41,22 @@
     <t>WESO</t>
   </si>
   <si>
-    <t>Description</t>
+    <t>English Description</t>
   </si>
   <si>
     <t>Description about WESO</t>
+  </si>
+  <si>
+    <t>Spanish Description</t>
+  </si>
+  <si>
+    <t>Descripcion sobre WESO</t>
+  </si>
+  <si>
+    <t>French Description</t>
+  </si>
+  <si>
+    <t>Description de WESO</t>
   </si>
   <si>
     <t>URL</t>
@@ -743,7 +755,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" customWidth="1" max="1" width="15.57"/>
+    <col min="1" customWidth="1" max="1" width="17.57"/>
     <col min="2" customWidth="1" max="2" width="33.43"/>
   </cols>
   <sheetData>
@@ -772,7 +784,7 @@
       <c t="s" s="2" r="A4">
         <v>5</v>
       </c>
-      <c t="s" s="3" r="B4">
+      <c t="s" s="2" r="B4">
         <v>6</v>
       </c>
     </row>
@@ -780,28 +792,28 @@
       <c t="s" s="2" r="A5">
         <v>7</v>
       </c>
-      <c t="s" s="3" r="B5">
+      <c t="s" s="2" r="B5">
         <v>8</v>
       </c>
     </row>
+    <row r="6">
+      <c t="s" s="2" r="A6">
+        <v>9</v>
+      </c>
+      <c t="s" s="3" r="B6">
+        <v>10</v>
+      </c>
+    </row>
     <row r="7">
-      <c t="s" s="1" r="A7">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8">
-      <c t="s" s="2" r="A8">
-        <v>10</v>
-      </c>
-      <c t="s" s="2" r="B8">
+      <c t="s" s="2" r="A7">
         <v>11</v>
       </c>
+      <c t="s" s="3" r="B7">
+        <v>12</v>
+      </c>
     </row>
     <row r="9">
-      <c t="s" s="2" r="A9">
-        <v>12</v>
-      </c>
-      <c t="s" s="2" r="B9">
+      <c t="s" s="1" r="A9">
         <v>13</v>
       </c>
     </row>
@@ -817,24 +829,40 @@
       <c t="s" s="2" r="A11">
         <v>16</v>
       </c>
-      <c t="s" s="3" r="B11">
+      <c t="s" s="2" r="B11">
         <v>17</v>
+      </c>
+    </row>
+    <row r="12">
+      <c t="s" s="2" r="A12">
+        <v>18</v>
+      </c>
+      <c t="s" s="2" r="B12">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13">
+      <c t="s" s="2" r="A13">
+        <v>20</v>
+      </c>
+      <c t="s" s="3" r="B13">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation sqref="B10" type="list">
+    <dataValidation sqref="B12" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
-    <hyperlink ref="B11" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId2"/>
+    <hyperlink ref="B13" r:id="rId3"/>
   </hyperlinks>
   <drawing r:id="rId4"/>
 </worksheet>
@@ -847,7 +875,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" customWidth="1" max="2" width="12.29"/>
+    <col min="2" customWidth="1" max="2" width="14.71"/>
     <col min="3" customWidth="1" max="3" width="12.86"/>
     <col min="4" customWidth="1" max="4" width="11.86"/>
     <col min="5" customWidth="1" max="5" width="16.71"/>
@@ -858,84 +886,84 @@
   <sheetData>
     <row r="1">
       <c t="s" s="2" r="A1">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c t="s" s="2" r="B1">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c t="s" s="2" r="C1">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c t="s" s="2" r="D1">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c t="s" s="2" r="E1">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c t="s" s="2" r="F1">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c t="s" s="2" r="G1">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c t="s" s="2" r="H1">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c t="s" s="2" r="I1">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c t="s" s="2" r="J1">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c t="s" s="2" r="K1">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c t="s" s="2" r="L1">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c t="s" s="2" r="M1">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="2" r="A2">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c t="s" s="2" r="B2">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c t="s" s="2" r="C2">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c t="s" s="2" r="D2">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c t="s" s="2" r="E2">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c t="s" s="2" r="F2">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c t="s" s="2" r="G2">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c t="s" s="2" r="H2">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c t="s" s="2" r="I2">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c t="s" s="2" r="J2">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c t="s" s="2" r="K2">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c s="2" r="L2">
         <v>1.0</v>
       </c>
       <c t="s" s="2" r="M2">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -966,16 +994,16 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c t="s" s="4" r="C1">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c t="s" s="4" r="D1">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c s="1" r="E1"/>
       <c s="1" r="F1"/>
@@ -986,7 +1014,7 @@
     </row>
     <row r="2">
       <c t="s" s="2" r="A2">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c s="1" r="B2">
         <v>20.1</v>
@@ -1005,7 +1033,7 @@
     </row>
     <row r="3">
       <c t="s" s="2" r="A3">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c s="1" r="B3">
         <v>20.2</v>
@@ -1021,7 +1049,7 @@
     </row>
     <row r="4">
       <c t="s" s="2" r="A4">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c s="1" r="B4">
         <v>20.3</v>
@@ -1037,7 +1065,7 @@
     </row>
     <row r="5">
       <c t="s" s="2" r="A5">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c s="1" r="B5">
         <v>20.400000000000002</v>
@@ -1053,7 +1081,7 @@
     </row>
     <row r="6">
       <c t="s" s="2" r="A6">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c s="1" r="B6">
         <v>20.500000000000004</v>
@@ -1062,14 +1090,14 @@
         <v>20.900000000000006</v>
       </c>
       <c t="s" s="1" r="D6">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c s="5" r="E6"/>
       <c s="5" r="F6"/>
     </row>
     <row r="7">
       <c t="s" s="2" r="A7">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c s="1" r="B7">
         <v>20.600000000000005</v>
@@ -1078,78 +1106,78 @@
         <v>21.000000000000007</v>
       </c>
       <c t="s" s="1" r="D7">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c s="5" r="E7"/>
       <c s="5" r="F7"/>
     </row>
     <row r="8">
       <c t="s" s="2" r="A8">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c s="1" r="B8">
         <v>20.700000000000006</v>
       </c>
       <c t="s" s="1" r="C8">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c t="s" s="1" r="D8">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c s="5" r="E8"/>
       <c s="5" r="F8"/>
     </row>
     <row r="9">
       <c t="s" s="2" r="A9">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c s="1" r="B9">
         <v>20.800000000000008</v>
       </c>
       <c t="s" s="1" r="C9">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c t="s" s="1" r="D9">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c s="5" r="E9"/>
       <c s="5" r="F9"/>
     </row>
     <row r="10">
       <c t="s" s="2" r="A10">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c s="1" r="B10">
         <v>20.90000000000001</v>
       </c>
       <c t="s" s="1" r="C10">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c t="s" s="1" r="D10">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c s="5" r="E10"/>
       <c s="5" r="F10"/>
     </row>
     <row r="11">
       <c t="s" s="2" r="A11">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c s="1" r="C11">
         <v>31.0</v>
       </c>
       <c t="s" s="1" r="D11">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c s="5" r="E11"/>
       <c s="5" r="F11"/>
     </row>
     <row r="12">
       <c t="s" s="2" r="A12">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c s="1" r="B12">
         <v>30.0</v>
@@ -1158,14 +1186,14 @@
         <v>20.3</v>
       </c>
       <c t="s" s="1" r="D12">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c s="5" r="E12"/>
       <c s="5" r="F12"/>
     </row>
     <row r="13">
       <c t="s" s="2" r="A13">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c s="1" r="B13">
         <v>30.0</v>
@@ -1174,20 +1202,20 @@
         <v>20.3</v>
       </c>
       <c t="s" s="1" r="D13">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c s="5" r="E13"/>
       <c s="5" r="F13"/>
     </row>
     <row r="14">
       <c t="s" s="2" r="A14">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c t="s" s="1" r="C14">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c s="1" r="D14">
         <v>15.0</v>
@@ -8620,657 +8648,657 @@
   <sheetData>
     <row r="1">
       <c t="s" s="2" r="A1">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="2" r="A2">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="2" r="A3">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="2" r="A4">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="2" r="A5">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="2" r="A6">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="2" r="A7">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="2" r="A8">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="2" r="A9">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="2" r="A10">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="2" r="A11">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="2" r="A12">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="2" r="A13">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="2" r="A14">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="2" r="A15">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="2" r="A16">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="2" r="A17">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18">
       <c t="s" s="2" r="A18">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19">
       <c t="s" s="2" r="A19">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20">
       <c t="s" s="2" r="A20">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21">
       <c t="s" s="2" r="A21">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22">
       <c t="s" s="2" r="A22">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23">
       <c t="s" s="2" r="A23">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24">
       <c t="s" s="2" r="A24">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25">
       <c t="s" s="2" r="A25">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26">
       <c t="s" s="2" r="A26">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27">
       <c t="s" s="2" r="A27">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28">
       <c t="s" s="2" r="A28">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29">
       <c t="s" s="2" r="A29">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30">
       <c t="s" s="2" r="A30">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31">
       <c t="s" s="2" r="A31">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32">
       <c t="s" s="2" r="A32">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33">
       <c t="s" s="2" r="A33">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34">
       <c t="s" s="2" r="A34">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35">
       <c t="s" s="2" r="A35">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36">
       <c t="s" s="2" r="A36">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37">
       <c t="s" s="2" r="A37">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38">
       <c t="s" s="2" r="A38">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39">
       <c t="s" s="2" r="A39">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40">
       <c t="s" s="2" r="A40">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41">
       <c t="s" s="2" r="A41">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42">
       <c t="s" s="2" r="A42">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43">
       <c t="s" s="2" r="A43">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44">
       <c t="s" s="2" r="A44">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45">
       <c t="s" s="2" r="A45">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46">
       <c t="s" s="2" r="A46">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47">
       <c t="s" s="2" r="A47">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="48">
       <c t="s" s="2" r="A48">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49">
       <c t="s" s="2" r="A49">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50">
       <c t="s" s="2" r="A50">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="51">
       <c t="s" s="2" r="A51">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="52">
       <c t="s" s="2" r="A52">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53">
       <c t="s" s="2" r="A53">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="54">
       <c t="s" s="2" r="A54">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="55">
       <c t="s" s="2" r="A55">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56">
       <c t="s" s="2" r="A56">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57">
       <c t="s" s="2" r="A57">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58">
       <c t="s" s="2" r="A58">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="59">
       <c t="s" s="2" r="A59">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60">
       <c t="s" s="2" r="A60">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="61">
       <c t="s" s="2" r="A61">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="62">
       <c t="s" s="2" r="A62">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="63">
       <c t="s" s="2" r="A63">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="64">
       <c t="s" s="2" r="A64">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="65">
       <c t="s" s="2" r="A65">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="66">
       <c t="s" s="2" r="A66">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="67">
       <c t="s" s="2" r="A67">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="68">
       <c t="s" s="2" r="A68">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="69">
       <c t="s" s="2" r="A69">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="70">
       <c t="s" s="2" r="A70">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="71">
       <c t="s" s="2" r="A71">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="72">
       <c t="s" s="2" r="A72">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="73">
       <c t="s" s="2" r="A73">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="74">
       <c t="s" s="2" r="A74">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="75">
       <c t="s" s="2" r="A75">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="76">
       <c t="s" s="2" r="A76">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="77">
       <c t="s" s="2" r="A77">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="78">
       <c t="s" s="2" r="A78">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="79">
       <c t="s" s="2" r="A79">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="80">
       <c t="s" s="2" r="A80">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="81">
       <c t="s" s="2" r="A81">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="82">
       <c t="s" s="2" r="A82">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="83">
       <c t="s" s="2" r="A83">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="84">
       <c t="s" s="2" r="A84">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="85">
       <c t="s" s="2" r="A85">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="86">
       <c t="s" s="2" r="A86">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="87">
       <c t="s" s="2" r="A87">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="88">
       <c t="s" s="2" r="A88">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="89">
       <c t="s" s="2" r="A89">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="90">
       <c t="s" s="2" r="A90">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="91">
       <c t="s" s="2" r="A91">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="92">
       <c t="s" s="2" r="A92">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="93">
       <c t="s" s="2" r="A93">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="94">
       <c t="s" s="2" r="A94">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="95">
       <c t="s" s="2" r="A95">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="96">
       <c t="s" s="2" r="A96">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="97">
       <c t="s" s="2" r="A97">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="98">
       <c t="s" s="2" r="A98">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="99">
       <c t="s" s="2" r="A99">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="100">
       <c t="s" s="2" r="A100">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="101">
       <c t="s" s="2" r="A101">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="102">
       <c t="s" s="2" r="A102">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="103">
       <c t="s" s="2" r="A103">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="104">
       <c t="s" s="2" r="A104">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="105">
       <c t="s" s="2" r="A105">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="106">
       <c t="s" s="2" r="A106">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="107">
       <c t="s" s="2" r="A107">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="108">
       <c t="s" s="2" r="A108">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="109">
       <c t="s" s="2" r="A109">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="110">
       <c t="s" s="2" r="A110">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="111">
       <c t="s" s="2" r="A111">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="112">
       <c t="s" s="2" r="A112">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="113">
       <c t="s" s="2" r="A113">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="114">
       <c t="s" s="2" r="A114">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="115">
       <c t="s" s="2" r="A115">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="116">
       <c t="s" s="2" r="A116">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="117">
       <c t="s" s="2" r="A117">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="118">
       <c t="s" s="2" r="A118">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="119">
       <c t="s" s="2" r="A119">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="120">
       <c t="s" s="2" r="A120">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="121">
       <c t="s" s="2" r="A121">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="122">
       <c t="s" s="2" r="A122">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="123">
       <c t="s" s="2" r="A123">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="124">
       <c t="s" s="2" r="A124">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="125">
       <c t="s" s="2" r="A125">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="126">
       <c t="s" s="2" r="A126">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="127">
       <c t="s" s="2" r="A127">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="128">
       <c t="s" s="2" r="A128">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="129">
       <c t="s" s="2" r="A129">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="130">
       <c t="s" s="2" r="A130">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="131">
       <c t="s" s="2" r="A131">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>